<commit_message>
Add Modify Files and New Files
</commit_message>
<xml_diff>
--- a/ProvarTraining/templates/All Objects.xlsx
+++ b/ProvarTraining/templates/All Objects.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chilly\ProvarP3\ProvarTraining\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D99851F-4DE5-4B5A-A567-0FACAD1F9BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A32EF91-501A-4A4C-B746-5A28E8131FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{52E0F12B-6321-4C30-9EC1-F7C3709814C2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="3" xr2:uid="{52E0F12B-6321-4C30-9EC1-F7C3709814C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Doctor__c" sheetId="13" r:id="rId1"/>
-    <sheet name="Appointment__c" sheetId="12" r:id="rId2"/>
-    <sheet name="Approved_Medical_Document__c" sheetId="11" r:id="rId3"/>
-    <sheet name="Denied_Medical_Document__c" sheetId="10" r:id="rId4"/>
-    <sheet name="Medical_History__c" sheetId="9" r:id="rId5"/>
-    <sheet name="Medical_History_Document__c" sheetId="8" r:id="rId6"/>
+    <sheet name="Medical_History__c" sheetId="9" r:id="rId2"/>
+    <sheet name="Medical_History_Document__c" sheetId="8" r:id="rId3"/>
+    <sheet name="Approved_Medical_Document__c" sheetId="11" r:id="rId4"/>
+    <sheet name="Denied_Medical_Document__c" sheetId="10" r:id="rId5"/>
+    <sheet name="Appointment__c" sheetId="12" r:id="rId6"/>
     <sheet name="Prescription__c" sheetId="7" r:id="rId7"/>
     <sheet name="Veteran__c" sheetId="3" r:id="rId8"/>
     <sheet name="Claim__c" sheetId="4" r:id="rId9"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="90">
   <si>
     <t>CreatedById</t>
   </si>
@@ -100,27 +100,9 @@
     <t>SystemModstamp</t>
   </si>
   <si>
-    <t>0054U00000ELBObQAP</t>
-  </si>
-  <si>
-    <t>2025-03-17T18:45:45.000Z</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
-    <t>a0i6C0000029lMpQAI</t>
-  </si>
-  <si>
-    <t>2025-03-18T20:33:31.000Z</t>
-  </si>
-  <si>
-    <t>Lama Su</t>
-  </si>
-  <si>
-    <t>Cloning Facility 64b9-yung</t>
-  </si>
-  <si>
     <t>Appointment_Date__c</t>
   </si>
   <si>
@@ -178,108 +160,12 @@
     <t>Related_Veteran__c</t>
   </si>
   <si>
-    <t>0054U00000ELBOgQAP</t>
-  </si>
-  <si>
-    <t>2025-03-17T21:48:33.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003EzkUUAS</t>
-  </si>
-  <si>
-    <t>Pat Fel Medical History</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlY7UAK</t>
-  </si>
-  <si>
-    <t>2025-03-18T19:46:36.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003EzkeUAC</t>
-  </si>
-  <si>
-    <t>Anakin Skywalker Medical History</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlWzUAK</t>
-  </si>
-  <si>
-    <t>2025-03-17T20:53:39.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003EzkFUAS</t>
-  </si>
-  <si>
-    <t>Bob Odenkirk\'s Medical History</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlXnUAK</t>
-  </si>
-  <si>
-    <t>2025-03-17T20:54:52.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003Ezk6UAC</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlXeUAK</t>
-  </si>
-  <si>
-    <t>0054U00000ELBNEQA5</t>
-  </si>
-  <si>
-    <t>2025-03-17T21:48:52.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003EzkZUAS</t>
-  </si>
-  <si>
-    <t>Test1 Test1 Medical History</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlYCUA0</t>
-  </si>
-  <si>
-    <t>2025-03-17T21:48:15.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003EzkPUAS</t>
-  </si>
-  <si>
-    <t>John McGyver Medical History</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlY2UAK</t>
-  </si>
-  <si>
-    <t>2025-03-17T21:46:11.000Z</t>
-  </si>
-  <si>
-    <t>a0D6C000003EzkKUAS</t>
-  </si>
-  <si>
-    <t>John McGoo Medical History</t>
-  </si>
-  <si>
-    <t>a0J6C000001PlXxUAK</t>
-  </si>
-  <si>
     <t>Related_Medical_History__c</t>
   </si>
   <si>
     <t>Uploaded_By__c</t>
   </si>
   <si>
-    <t>2025-03-19T20:50:14.000Z</t>
-  </si>
-  <si>
-    <t>a0j6C000002NFlgQAG</t>
-  </si>
-  <si>
-    <t>Anakin Skywalker Medical History Documents</t>
-  </si>
-  <si>
     <t>Dispense_Amount__c</t>
   </si>
   <si>
@@ -380,6 +266,57 @@
   </si>
   <si>
     <t>111-22-3333</t>
+  </si>
+  <si>
+    <t>Phone_Number__c</t>
+  </si>
+  <si>
+    <t>bristlje@gmail.com</t>
+  </si>
+  <si>
+    <t>999-888-7777</t>
+  </si>
+  <si>
+    <t>Julius</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Dr. Julius No</t>
+  </si>
+  <si>
+    <t>SPECTRE</t>
+  </si>
+  <si>
+    <t>Incomplete Information</t>
+  </si>
+  <si>
+    <t>Missing Key info from Document</t>
+  </si>
+  <si>
+    <t>General Physical</t>
+  </si>
+  <si>
+    <t>Medical Exam</t>
+  </si>
+  <si>
+    <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Bruce Willis's Medical History</t>
+  </si>
+  <si>
+    <t>Bruce Willis Medical History Documents</t>
+  </si>
+  <si>
+    <t>Bruce Willis Approved Medical History Documents</t>
+  </si>
+  <si>
+    <t>Bruce Willis Denied Medical History Documents</t>
+  </si>
+  <si>
+    <t>Valid Documents</t>
   </si>
 </sst>
 </file>
@@ -424,9 +361,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,10 +381,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,34 +700,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F5A193-A0E4-42B8-8C35-9A1E7383B04E}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -837,57 +775,63 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
       <c r="K2">
-        <v>32.311008999999999</v>
+        <v>18.059764925973099</v>
       </c>
       <c r="L2">
-        <v>-64.746151999999995</v>
+        <v>-76.576813245939405</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="P2" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>75</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{58F094A6-D6E0-4A69-9724-F74E6889D83A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -932,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -944,7 +888,7 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
         <v>16</v>
@@ -985,19 +929,19 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1015,7 +959,7 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
@@ -1064,7 +1008,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1076,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1085,7 +1029,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -1106,76 +1050,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49542423-4AA9-4300-886A-01F2BE24E67D}">
-  <dimension ref="A1:U1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27ED704-C631-4756-AC90-D0F097FE326C}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="b">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>32</v>
+      <c r="K2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1184,61 +1139,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CB6B3B-FCDB-4CA8-8487-9FDFD49F2BF4}">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED2E72C-9D09-4F6A-A9A4-C4BCA889B865}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD211"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1247,31 +1214,50 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80DA693-90C9-420B-95F1-7CD0A81A7963}">
-  <dimension ref="A1:Q1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CB6B3B-FCDB-4CA8-8487-9FDFD49F2BF4}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1280,7 +1266,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -1295,16 +1281,21 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O1" t="s">
         <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1313,16 +1304,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27ED704-C631-4756-AC90-D0F097FE326C}">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80DA693-90C9-420B-95F1-7CD0A81A7963}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q44:Q45"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1333,306 +1342,58 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" t="s">
+        <v>81</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>63</v>
-      </c>
-      <c r="O6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" t="s">
-        <v>71</v>
-      </c>
-      <c r="O8" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1641,87 +1402,112 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED2E72C-9D09-4F6A-A9A4-C4BCA889B865}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49542423-4AA9-4300-886A-01F2BE24E67D}">
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
-        <v>73</v>
+      <c r="U1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1748,31 +1534,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -1793,16 +1579,16 @@
         <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="T1" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="U1" t="s">
         <v>16</v>
       </c>
       <c r="V1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E55919-3734-4078-8F52-612E1871CF5B}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1854,16 +1640,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1872,7 +1658,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
@@ -1881,16 +1667,16 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="N1" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="O1" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="P1" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="Q1" t="s">
         <v>13</v>
@@ -1899,10 +1685,10 @@
         <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="T1" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="U1" t="s">
         <v>16</v>
@@ -1910,25 +1696,25 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="M2" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="T2" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1975,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1984,7 +1770,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -1999,7 +1785,7 @@
         <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="M1" t="s">
         <v>16</v>
@@ -2011,6 +1797,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="615783ef-0f63-4cad-b62c-df58d527f7fb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010026489E7EE3241043AA20E76F34F7FC65" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9e07a6230b0c1d7d3c3286cea7bd727">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="615783ef-0f63-4cad-b62c-df58d527f7fb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e17c25d355ca5f9125709803ae213077" ns3:_="">
     <xsd:import namespace="615783ef-0f63-4cad-b62c-df58d527f7fb"/>
@@ -2192,7 +1986,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2201,15 +1995,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="615783ef-0f63-4cad-b62c-df58d527f7fb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27A3C6C-5772-4DD5-9FF2-37167BBB9C6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="615783ef-0f63-4cad-b62c-df58d527f7fb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{473B2FE8-82B8-4843-8188-CDB62D9DDBA9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2227,26 +2029,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E74623D-9A51-4C4C-8173-6A83747C3474}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27A3C6C-5772-4DD5-9FF2-37167BBB9C6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="615783ef-0f63-4cad-b62c-df58d527f7fb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>